<commit_message>
Add logistic curve to POD paper fig
</commit_message>
<xml_diff>
--- a/00_raw_reports/GHG_Stage1_submitted-2022-11-21.xlsx
+++ b/00_raw_reports/GHG_Stage1_submitted-2022-11-21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sea/PycharmProjects/CRF22_Airplanes/00_raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sea/PycharmProjects/CRF22_Airplanes/00_raw_reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C116ECA-7E27-E94F-928E-CEC245CDE8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03596467-E050-324D-AAD9-938DA266CA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20040" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -1145,7 +1145,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
     <numFmt numFmtId="166" formatCode="0.0000000"/>
-    <numFmt numFmtId="168" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1571,16 +1571,16 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2110,8 +2110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2244,7 +2244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S483"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>

</xml_diff>

<commit_message>
Adjust PoD plot to have 3 kgh bin width
</commit_message>
<xml_diff>
--- a/00_raw_reports/GHG_Stage1_submitted-2022-11-21.xlsx
+++ b/00_raw_reports/GHG_Stage1_submitted-2022-11-21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sea/PycharmProjects/CRF22_Airplanes/00_raw_reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03596467-E050-324D-AAD9-938DA266CA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE886713-E59D-2F45-AFB9-66BF37748DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2110,8 +2110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>